<commit_message>
CCDB-318: Using a new separator for the absolute slot path ">>"
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/slots-import-creation-fails.xlsx
+++ b/conf-core/src/test/resources/dataloader/slots-import-creation-fails.xlsx
@@ -234,11 +234,6 @@
     <t>Path not found</t>
   </si>
   <si>
-    <t>IMPORT_TEST_2
-IMPORT_TEST_3
-IMPORT_TEST_5</t>
-  </si>
-  <si>
     <t>Required install missing</t>
   </si>
   <si>
@@ -333,6 +328,9 @@
   </si>
   <si>
     <t>INSTALL DEVICE</t>
+  </si>
+  <si>
+    <t>IMPORT_TEST_2&gt;&gt;IMPORT_TEST_3&gt;&gt;IMPORT_TEST_5</t>
   </si>
 </sst>
 </file>
@@ -480,13 +478,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,7 +819,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -892,10 +888,10 @@
     </row>
     <row r="7" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -964,7 +960,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -978,7 +974,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,7 +988,7 @@
         <v>59</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>55</v>
@@ -1009,7 +1005,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>59</v>
@@ -1026,7 +1022,7 @@
         <v>60</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>30</v>
@@ -1040,13 +1036,13 @@
         <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>30</v>
@@ -1060,13 +1056,13 @@
         <v>24</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>30</v>
@@ -1083,10 +1079,10 @@
         <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>41</v>
@@ -1103,10 +1099,10 @@
         <v>31</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>41</v>
@@ -1114,7 +1110,7 @@
     </row>
     <row r="20" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>24</v>
@@ -1123,7 +1119,7 @@
         <v>31</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
         <v>30</v>
@@ -1137,25 +1133,25 @@
     </row>
     <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
         <v>30</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1164,7 +1160,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1255,7 +1251,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>62</v>
@@ -1272,7 +1268,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>31</v>
@@ -1315,7 +1311,7 @@
         <v>40</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>41</v>
@@ -1335,7 +1331,7 @@
         <v>46</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H32" s="3"/>
     </row>
@@ -1350,10 +1346,10 @@
         <v>30</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1370,7 +1366,7 @@
         <v>43</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>42</v>
@@ -1390,7 +1386,7 @@
         <v>47</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>48</v>
@@ -1410,7 +1406,7 @@
         <v>49</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>48</v>
@@ -1430,7 +1426,7 @@
         <v>40</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>48</v>
@@ -1450,7 +1446,7 @@
         <v>50</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>41</v>
@@ -1470,7 +1466,7 @@
         <v>49</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>48</v>
@@ -1478,7 +1474,7 @@
     </row>
     <row r="40" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>24</v>
@@ -1498,7 +1494,7 @@
     </row>
     <row r="41" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>24</v>
@@ -1518,7 +1514,7 @@
     </row>
     <row r="42" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>24</v>
@@ -1541,7 +1537,7 @@
     </row>
     <row r="43" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>24</v>
@@ -1550,7 +1546,7 @@
         <v>31</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F43" t="s">
         <v>30</v>
@@ -1564,7 +1560,7 @@
     </row>
     <row r="44" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>24</v>
@@ -1573,7 +1569,7 @@
         <v>31</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" t="s">
         <v>30</v>
@@ -1587,7 +1583,7 @@
     </row>
     <row r="45" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>23</v>
@@ -1616,7 +1612,7 @@
         <v>24</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>62</v>
@@ -1633,7 +1629,7 @@
         <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>64</v>
@@ -1653,7 +1649,7 @@
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>67</v>
@@ -1665,7 +1661,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>25</v>
       </c>
@@ -1673,7 +1669,7 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>69</v>
@@ -1681,25 +1677,25 @@
       <c r="E49" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>71</v>
+      <c r="F49" s="10" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F50" t="s">
         <v>30</v>
@@ -1707,71 +1703,71 @@
     </row>
     <row r="51" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F51" t="s">
         <v>30</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
         <v>30</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F53" t="s">
         <v>30</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1856,7 +1852,7 @@
       <c r="B66" s="4"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="9"/>
+      <c r="F66" s="8"/>
     </row>
     <row r="67" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>

</xml_diff>